<commit_message>
Using my fork of scraper which allows passing of language filter and max review count.
</commit_message>
<xml_diff>
--- a/scraper/places_list.xlsx
+++ b/scraper/places_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\piebm\source\repos\google-maps-review-model\scraper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1984A88F-4401-494D-A8D5-2B646105F9D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A367F9B1-931F-4F64-97B6-74E3B80F4432}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -660,7 +660,7 @@
   <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F4"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1169,35 +1169,9 @@
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="G3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="G4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="G5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="G6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="G7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="G8" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="G9" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="G10" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="G11" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="G12" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="G13" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="G14" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="G15" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="G16" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="G17" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="G18" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="G19" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="G20" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="G21" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="G22" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="G23" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="G24" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="G25" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:AQ1 A5:AQ302 A2:E4 G2:AQ4" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:G1 A6:G25 A2:E5 G2:G5" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>